<commit_message>
Add description of natural noise temporal NLM processing
</commit_message>
<xml_diff>
--- a/Summary table.xlsx
+++ b/Summary table.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
   <si>
     <t>Битрейт</t>
   </si>
@@ -130,20 +130,25 @@
   <si>
     <t>search_size</t>
   </si>
-  <si>
-    <t>Расчёты производились несколько иначе по сравнению с предыдущими алгоритмами</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -190,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,14 +214,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="23">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -430,75 +429,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="dotted">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dotted">
-        <color auto="1"/>
-      </right>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dotted">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dotted">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -513,133 +450,172 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -651,49 +627,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1033,22 +976,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="35" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="48" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
+      <c r="A3" s="42"/>
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1064,7 +1007,7 @@
       <c r="F3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="49"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1073,19 +1016,19 @@
       <c r="B4" s="3">
         <v>150</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="50">
         <v>0.01</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="50">
         <v>30</v>
       </c>
       <c r="E4" s="2">
         <v>3</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="50">
         <v>4.0190000000000001</v>
       </c>
     </row>
@@ -1096,13 +1039,13 @@
       <c r="B5" s="3">
         <v>150</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="2">
         <v>5</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="38"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="51"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -1111,13 +1054,13 @@
       <c r="B6" s="3">
         <v>150</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="2">
         <v>9</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="38"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="51"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -1126,13 +1069,13 @@
       <c r="B7" s="3">
         <v>200</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
       <c r="E7" s="2">
         <v>3</v>
       </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="38"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="51"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -1141,13 +1084,13 @@
       <c r="B8" s="3">
         <v>200</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="2">
         <v>5</v>
       </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="39"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="12" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1167,18 +1110,18 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2">
@@ -1187,7 +1130,7 @@
       <c r="C14" s="2">
         <v>513</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="45" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="9"/>
@@ -1195,42 +1138,42 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="2">
         <v>32</v>
       </c>
       <c r="C15" s="2">
         <v>106</v>
       </c>
-      <c r="D15" s="50"/>
+      <c r="D15" s="46"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="2">
         <v>40</v>
       </c>
       <c r="C16" s="2">
         <v>35</v>
       </c>
-      <c r="D16" s="51"/>
+      <c r="D16" s="47"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="41">
+      <c r="A18" s="37">
         <v>95</v>
       </c>
       <c r="B18" s="2">
@@ -1246,7 +1189,7 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="2">
         <v>32</v>
       </c>
@@ -1260,7 +1203,7 @@
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="47"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="10">
         <v>40</v>
       </c>
@@ -1274,7 +1217,7 @@
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39">
+      <c r="A21" s="36">
         <v>98</v>
       </c>
       <c r="B21" s="7">
@@ -1290,7 +1233,7 @@
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="2">
         <v>32</v>
       </c>
@@ -1303,7 +1246,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="47"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="10">
         <v>40</v>
       </c>
@@ -1316,7 +1259,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="39">
+      <c r="A24" s="36">
         <v>173</v>
       </c>
       <c r="B24" s="7">
@@ -1331,7 +1274,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="2">
         <v>32</v>
       </c>
@@ -1344,7 +1287,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="2">
         <v>40</v>
       </c>
@@ -1358,6 +1301,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="C4:C8"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="F4:F8"/>
+    <mergeCell ref="G4:G8"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B2:F2"/>
@@ -1367,11 +1315,6 @@
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="D14:D16"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="C4:C8"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="F4:F8"/>
-    <mergeCell ref="G4:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1382,7 +1325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -1401,50 +1344,50 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="56" t="s">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="53" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
+      <c r="A3" s="42"/>
       <c r="B3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55" t="s">
+      <c r="D3" s="59"/>
+      <c r="E3" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="56"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="53"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>8</v>
       </c>
-      <c r="B4" s="52">
+      <c r="B4" s="56">
         <v>0.8</v>
       </c>
-      <c r="C4" s="57">
+      <c r="C4" s="54">
         <v>5</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="57">
+      <c r="D4" s="55"/>
+      <c r="E4" s="54">
         <v>6</v>
       </c>
-      <c r="F4" s="58"/>
+      <c r="F4" s="55"/>
       <c r="G4" s="3">
         <v>30.92</v>
       </c>
@@ -1453,15 +1396,15 @@
       <c r="A5" s="20">
         <v>9</v>
       </c>
-      <c r="B5" s="53"/>
-      <c r="C5" s="57">
+      <c r="B5" s="57"/>
+      <c r="C5" s="54">
         <v>5</v>
       </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="57">
+      <c r="D5" s="55"/>
+      <c r="E5" s="54">
         <v>10</v>
       </c>
-      <c r="F5" s="58"/>
+      <c r="F5" s="55"/>
       <c r="G5" s="3">
         <v>30.93</v>
       </c>
@@ -1470,15 +1413,15 @@
       <c r="A6" s="21">
         <v>10</v>
       </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="57">
+      <c r="B6" s="57"/>
+      <c r="C6" s="54">
         <v>7</v>
       </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="57">
+      <c r="D6" s="55"/>
+      <c r="E6" s="54">
         <v>6</v>
       </c>
-      <c r="F6" s="58"/>
+      <c r="F6" s="55"/>
       <c r="G6" s="3">
         <v>30.68</v>
       </c>
@@ -1487,15 +1430,15 @@
       <c r="A7" s="14">
         <v>11</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="57">
+      <c r="B7" s="58"/>
+      <c r="C7" s="54">
         <v>7</v>
       </c>
-      <c r="D7" s="58"/>
-      <c r="E7" s="57">
+      <c r="D7" s="55"/>
+      <c r="E7" s="54">
         <v>10</v>
       </c>
-      <c r="F7" s="58"/>
+      <c r="F7" s="55"/>
       <c r="G7" s="3">
         <v>30.66</v>
       </c>
@@ -1507,14 +1450,14 @@
       <c r="B8" s="19">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C8" s="57">
+      <c r="C8" s="54">
         <v>5</v>
       </c>
-      <c r="D8" s="58"/>
-      <c r="E8" s="57">
+      <c r="D8" s="55"/>
+      <c r="E8" s="54">
         <v>6</v>
       </c>
-      <c r="F8" s="58"/>
+      <c r="F8" s="55"/>
       <c r="G8" s="3">
         <v>30.84</v>
       </c>
@@ -1546,21 +1489,21 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="F13" s="48" t="s">
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="F13" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="12">
@@ -1569,10 +1512,10 @@
       <c r="C14" s="12">
         <v>13498</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="42" t="s">
+      <c r="F14" s="38" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="24">
@@ -1581,62 +1524,62 @@
       <c r="H14" s="24">
         <v>1692</v>
       </c>
-      <c r="I14" s="49" t="s">
+      <c r="I14" s="45" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="12">
         <v>32</v>
       </c>
       <c r="C15" s="12">
         <v>2778</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="F15" s="42"/>
+      <c r="D15" s="46"/>
+      <c r="F15" s="38"/>
       <c r="G15" s="24">
         <v>32</v>
       </c>
       <c r="H15" s="24">
         <v>323</v>
       </c>
-      <c r="I15" s="50"/>
+      <c r="I15" s="46"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="12">
         <v>40</v>
       </c>
       <c r="C16" s="12">
         <v>76</v>
       </c>
-      <c r="D16" s="51"/>
-      <c r="F16" s="42"/>
+      <c r="D16" s="47"/>
+      <c r="F16" s="38"/>
       <c r="G16" s="24">
         <v>40</v>
       </c>
       <c r="H16" s="24">
         <v>60</v>
       </c>
-      <c r="I16" s="51"/>
+      <c r="I16" s="47"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="F17" s="48" t="s">
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="F17" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="41">
+      <c r="A18" s="37">
         <v>8</v>
       </c>
       <c r="B18" s="12">
@@ -1649,7 +1592,7 @@
         <f>1-C18/C14</f>
         <v>0.76789153948733146</v>
       </c>
-      <c r="F18" s="41">
+      <c r="F18" s="37">
         <v>8</v>
       </c>
       <c r="G18" s="24">
@@ -1664,7 +1607,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="12">
         <v>32</v>
       </c>
@@ -1675,7 +1618,7 @@
         <f t="shared" ref="D19:D20" si="0">1-C19/C15</f>
         <v>0.82001439884809213</v>
       </c>
-      <c r="F19" s="41"/>
+      <c r="F19" s="37"/>
       <c r="G19" s="24">
         <v>32</v>
       </c>
@@ -1688,7 +1631,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="47"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="15">
         <v>40</v>
       </c>
@@ -1699,7 +1642,7 @@
         <f t="shared" si="0"/>
         <v>0.22368421052631582</v>
       </c>
-      <c r="F20" s="47"/>
+      <c r="F20" s="43"/>
       <c r="G20" s="25">
         <v>40</v>
       </c>
@@ -1712,7 +1655,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39">
+      <c r="A21" s="36">
         <v>9</v>
       </c>
       <c r="B21" s="11">
@@ -1725,7 +1668,7 @@
         <f>1-C21/C14</f>
         <v>0.79226552081789892</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F21" s="36">
         <v>9</v>
       </c>
       <c r="G21" s="23">
@@ -1740,7 +1683,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="12">
         <v>32</v>
       </c>
@@ -1751,7 +1694,7 @@
         <f t="shared" ref="D22:D23" si="2">1-C22/C15</f>
         <v>0.83585313174946008</v>
       </c>
-      <c r="F22" s="41"/>
+      <c r="F22" s="37"/>
       <c r="G22" s="24">
         <v>32</v>
       </c>
@@ -1764,7 +1707,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="47"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="15">
         <v>40</v>
       </c>
@@ -1775,7 +1718,7 @@
         <f t="shared" si="2"/>
         <v>0.23684210526315785</v>
       </c>
-      <c r="F23" s="47"/>
+      <c r="F23" s="43"/>
       <c r="G23" s="25">
         <v>40</v>
       </c>
@@ -1788,7 +1731,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="39">
+      <c r="A24" s="36">
         <v>12</v>
       </c>
       <c r="B24" s="11">
@@ -1801,7 +1744,7 @@
         <f>1-C24/C14</f>
         <v>0.85353385686768413</v>
       </c>
-      <c r="F24" s="39">
+      <c r="F24" s="36">
         <v>12</v>
       </c>
       <c r="G24" s="23">
@@ -1816,7 +1759,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="12">
         <v>32</v>
       </c>
@@ -1827,7 +1770,7 @@
         <f t="shared" ref="D25:D26" si="4">1-C25/C15</f>
         <v>0.88048956083513319</v>
       </c>
-      <c r="F25" s="41"/>
+      <c r="F25" s="37"/>
       <c r="G25" s="24">
         <v>32</v>
       </c>
@@ -1840,7 +1783,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="12">
         <v>40</v>
       </c>
@@ -1851,7 +1794,7 @@
         <f t="shared" si="4"/>
         <v>0.28947368421052633</v>
       </c>
-      <c r="F26" s="41"/>
+      <c r="F26" s="37"/>
       <c r="G26" s="24">
         <v>40</v>
       </c>
@@ -1865,20 +1808,11 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -1890,11 +1824,20 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1903,10 +1846,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G23"/>
+  <dimension ref="A2:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,26 +1858,28 @@
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="65" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="42"/>
       <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
@@ -1947,271 +1892,426 @@
       <c r="E3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="36"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="29">
+      <c r="F3" s="66"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="28">
         <v>1</v>
       </c>
-      <c r="B4" s="52">
+      <c r="B4" s="56">
         <v>5</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="28">
         <v>1.1499999999999999</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="37">
         <v>5</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="27">
         <v>13</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="29">
         <v>29.06</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="33">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="30">
         <v>2</v>
       </c>
-      <c r="B5" s="53"/>
-      <c r="C5" s="29">
+      <c r="B5" s="57"/>
+      <c r="C5" s="28">
         <v>0.8</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="65">
+      <c r="D5" s="37"/>
+      <c r="E5" s="60">
         <v>21</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="29">
         <v>28.86</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="33">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="30">
         <v>3</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="29">
+      <c r="B6" s="58"/>
+      <c r="C6" s="28">
         <v>3</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="32">
+      <c r="D6" s="37"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="29">
         <v>26.18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="35" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="F9" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="F10" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="33">
         <v>24</v>
       </c>
-      <c r="C11" s="29">
-        <v>57370</v>
-      </c>
-      <c r="D11" s="49" t="s">
+      <c r="C11" s="33">
+        <v>13498</v>
+      </c>
+      <c r="D11" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="60"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
-      <c r="B12" s="29">
+      <c r="F11" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="33">
+        <v>24</v>
+      </c>
+      <c r="H11" s="33">
+        <v>1692</v>
+      </c>
+      <c r="I11" s="62" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
+      <c r="B12" s="33">
         <v>32</v>
       </c>
-      <c r="C12" s="29">
-        <v>11685</v>
-      </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="62"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
-      <c r="B13" s="29">
+      <c r="C12" s="33">
+        <v>2778</v>
+      </c>
+      <c r="D12" s="63"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="33">
+        <v>32</v>
+      </c>
+      <c r="H12" s="33">
+        <v>323</v>
+      </c>
+      <c r="I12" s="63"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
+      <c r="B13" s="33">
         <v>40</v>
       </c>
-      <c r="C13" s="29">
-        <v>324</v>
-      </c>
-      <c r="D13" s="51"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="64"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
+      <c r="C13" s="33">
+        <v>76</v>
+      </c>
+      <c r="D13" s="64"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="33">
+        <v>40</v>
+      </c>
+      <c r="H13" s="33">
+        <v>60</v>
+      </c>
+      <c r="I13" s="64"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="41">
-        <v>8</v>
-      </c>
-      <c r="B15" s="29">
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="F14" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="37">
+        <v>1</v>
+      </c>
+      <c r="B15" s="33">
         <v>24</v>
       </c>
-      <c r="C15" s="29">
-        <v>10988</v>
+      <c r="C15" s="33">
+        <v>2566</v>
       </c>
       <c r="D15" s="16">
         <f>1-C15/C11</f>
-        <v>0.80847132647725295</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="29">
+        <v>0.80989776263150093</v>
+      </c>
+      <c r="F15" s="37">
+        <v>1</v>
+      </c>
+      <c r="G15" s="33">
+        <v>24</v>
+      </c>
+      <c r="H15" s="33">
+        <v>1681</v>
+      </c>
+      <c r="I15" s="16">
+        <f>1-H15/H11</f>
+        <v>6.5011820330969083E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="37"/>
+      <c r="B16" s="33">
         <v>32</v>
       </c>
-      <c r="C16" s="29">
-        <v>1209</v>
+      <c r="C16" s="33">
+        <v>282</v>
       </c>
       <c r="D16" s="18">
         <f t="shared" ref="D16:D17" si="0">1-C16/C12</f>
-        <v>0.89653401797175869</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="47"/>
-      <c r="B17" s="30">
+        <v>0.89848812095032393</v>
+      </c>
+      <c r="F16" s="37"/>
+      <c r="G16" s="33">
+        <v>32</v>
+      </c>
+      <c r="H16" s="33">
+        <v>314</v>
+      </c>
+      <c r="I16" s="18">
+        <f t="shared" ref="I16:I17" si="1">1-H16/H12</f>
+        <v>2.786377708978327E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="43"/>
+      <c r="B17" s="34">
         <v>40</v>
       </c>
-      <c r="C17" s="30">
-        <v>230</v>
+      <c r="C17" s="34">
+        <v>53</v>
       </c>
       <c r="D17" s="17">
         <f t="shared" si="0"/>
-        <v>0.29012345679012341</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39">
-        <v>9</v>
-      </c>
-      <c r="B18" s="27">
+        <v>0.30263157894736847</v>
+      </c>
+      <c r="F17" s="43"/>
+      <c r="G17" s="34">
+        <v>40</v>
+      </c>
+      <c r="H17" s="34">
+        <v>59</v>
+      </c>
+      <c r="I17" s="17">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666718E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36">
+        <v>2</v>
+      </c>
+      <c r="B18" s="32">
         <v>24</v>
       </c>
-      <c r="C18" s="29">
-        <v>19069</v>
+      <c r="C18" s="33">
+        <v>4453</v>
       </c>
       <c r="D18" s="22">
         <f>1-C18/C11</f>
-        <v>0.66761373540177793</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="29">
+        <v>0.67009927396651348</v>
+      </c>
+      <c r="F18" s="36">
+        <v>2</v>
+      </c>
+      <c r="G18" s="32">
+        <v>24</v>
+      </c>
+      <c r="H18" s="33">
+        <v>1687</v>
+      </c>
+      <c r="I18" s="22">
+        <f>1-H18/H11</f>
+        <v>2.9550827423168169E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
+      <c r="B19" s="33">
         <v>32</v>
       </c>
-      <c r="C19" s="29">
-        <v>2485</v>
+      <c r="C19" s="33">
+        <v>580</v>
       </c>
       <c r="D19" s="18">
-        <f t="shared" ref="D19:D20" si="1">1-C19/C12</f>
-        <v>0.78733418913136499</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="47"/>
-      <c r="B20" s="30">
+        <f t="shared" ref="D19:D20" si="2">1-C19/C12</f>
+        <v>0.79121670266378685</v>
+      </c>
+      <c r="F19" s="37"/>
+      <c r="G19" s="33">
+        <v>32</v>
+      </c>
+      <c r="H19" s="33">
+        <v>316</v>
+      </c>
+      <c r="I19" s="18">
+        <f t="shared" ref="I19:I20" si="3">1-H19/H12</f>
+        <v>2.1671826625387025E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="43"/>
+      <c r="B20" s="34">
         <v>40</v>
       </c>
-      <c r="C20" s="30">
-        <v>263</v>
+      <c r="C20" s="34">
+        <v>61</v>
       </c>
       <c r="D20" s="17">
-        <f t="shared" si="1"/>
-        <v>0.18827160493827155</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39">
-        <v>12</v>
-      </c>
-      <c r="B21" s="27">
+        <f t="shared" si="2"/>
+        <v>0.19736842105263153</v>
+      </c>
+      <c r="F20" s="43"/>
+      <c r="G20" s="34">
+        <v>40</v>
+      </c>
+      <c r="H20" s="34">
+        <v>59</v>
+      </c>
+      <c r="I20" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666718E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="36">
+        <v>3</v>
+      </c>
+      <c r="B21" s="32">
         <v>24</v>
       </c>
-      <c r="C21" s="29">
-        <v>5657</v>
+      <c r="C21" s="33">
+        <v>1321</v>
       </c>
       <c r="D21" s="22">
         <f>1-C21/C11</f>
-        <v>0.90139445703329268</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="29">
+        <v>0.9021336494295451</v>
+      </c>
+      <c r="F21" s="36">
+        <v>3</v>
+      </c>
+      <c r="G21" s="32">
+        <v>24</v>
+      </c>
+      <c r="H21" s="33">
+        <v>1576</v>
+      </c>
+      <c r="I21" s="68">
+        <f>1-H21/H11</f>
+        <v>6.8557919621749397E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="37"/>
+      <c r="B22" s="33">
         <v>32</v>
       </c>
-      <c r="C22" s="29">
-        <v>492</v>
+      <c r="C22" s="33">
+        <v>115</v>
       </c>
       <c r="D22" s="18">
-        <f t="shared" ref="D22:D23" si="2">1-C22/C12</f>
-        <v>0.95789473684210524</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="29">
+        <f t="shared" ref="D22:D23" si="4">1-C22/C12</f>
+        <v>0.95860331173506119</v>
+      </c>
+      <c r="F22" s="37"/>
+      <c r="G22" s="33">
+        <v>32</v>
+      </c>
+      <c r="H22" s="33">
+        <v>303</v>
+      </c>
+      <c r="I22" s="67">
+        <f t="shared" ref="I22:I23" si="5">1-H22/H12</f>
+        <v>6.1919504643962897E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="37"/>
+      <c r="B23" s="33">
         <v>40</v>
       </c>
-      <c r="C23" s="29">
-        <v>169</v>
+      <c r="C23" s="33">
+        <v>39</v>
       </c>
       <c r="D23" s="16">
-        <f t="shared" si="2"/>
-        <v>0.47839506172839508</v>
+        <f t="shared" si="4"/>
+        <v>0.48684210526315785</v>
+      </c>
+      <c r="F23" s="37"/>
+      <c r="G23" s="33">
+        <v>40</v>
+      </c>
+      <c r="H23" s="33">
+        <v>58</v>
+      </c>
+      <c r="I23" s="16">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333326E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="20">
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="F21:F23"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="D4:D6"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="F11:G13"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>